<commit_message>
Fix Code Bugs and Add Field For Invoice Generator
</commit_message>
<xml_diff>
--- a/InvoiceLogTemplate (1).xlsx
+++ b/InvoiceLogTemplate (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.demosthenous\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My OFFICE\PROJECTS\Freelauncing Agency\Upwork\DemosthenisD\TeamCY-main\Changes-2\Updated_Invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B264C9F0-845C-42D2-B3D8-E27EE7815137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4C6BF9-0481-42CE-BE94-8DBC579DE33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLogTemplate" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="157">
   <si>
     <t>Year</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>Partially Biled</t>
+  </si>
+  <si>
+    <t>demo adress</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -619,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -634,8 +637,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,9 +960,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,12 +1018,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2024</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -1095,18 +1098,18 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1547,12 +1550,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>85</v>
       </c>
@@ -1560,27 +1563,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>85</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>85</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>85</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>85</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>85</v>
       </c>
@@ -1620,27 +1623,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>85</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>85</v>
       </c>
@@ -1656,7 +1659,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>85</v>
       </c>
@@ -1664,7 +1667,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>40</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>40</v>
       </c>
@@ -1688,12 +1691,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>85</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>22</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>22</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>82</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>85</v>
       </c>
@@ -1750,24 +1753,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C84102-4356-4026-B842-2F4342558093}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.20703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.89453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.20703125" customWidth="1"/>
-    <col min="8" max="8" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1794,7 +1797,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1812,12 +1815,15 @@
         <f>VLOOKUP($D2,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G2" t="s">
+        <v>156</v>
+      </c>
       <c r="H2" s="7" t="str">
         <f>VLOOKUP($D2,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1839,12 +1845,15 @@
         <f>VLOOKUP($D3,Table1[],3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G3" t="s">
+        <v>156</v>
+      </c>
       <c r="H3" s="7" t="str">
         <f>VLOOKUP($D3,Table1[],4,FALSE)</f>
         <v>Template-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1866,12 +1875,15 @@
         <f>VLOOKUP($D4,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G4" t="s">
+        <v>156</v>
+      </c>
       <c r="H4" s="7" t="str">
         <f>VLOOKUP($D4,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -1893,12 +1905,15 @@
         <f>VLOOKUP($D5,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
       <c r="H5" s="7" t="str">
         <f>VLOOKUP($D5,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1920,12 +1935,15 @@
         <f>VLOOKUP($D6,Table1[],3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G6" t="s">
+        <v>156</v>
+      </c>
       <c r="H6" s="7" t="str">
         <f>VLOOKUP($D6,Table1[],4,FALSE)</f>
         <v>Template-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
@@ -1946,12 +1964,15 @@
         <f>VLOOKUP($D7,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G7" t="s">
+        <v>156</v>
+      </c>
       <c r="H7" s="7" t="str">
         <f>VLOOKUP($D7,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>102</v>
       </c>
@@ -1972,12 +1993,15 @@
         <f>VLOOKUP($D8,Table1[],3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G8" t="s">
+        <v>156</v>
+      </c>
       <c r="H8" s="7" t="str">
         <f>VLOOKUP($D8,Table1[],4,FALSE)</f>
         <v>Template-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -1999,12 +2023,15 @@
         <f>VLOOKUP($D9,Table1[],3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G9" t="s">
+        <v>156</v>
+      </c>
       <c r="H9" s="7" t="str">
         <f>VLOOKUP($D9,Table1[],4,FALSE)</f>
         <v>Template-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
@@ -2026,12 +2053,15 @@
         <f>VLOOKUP($D10,Table1[],3,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G10" t="s">
+        <v>156</v>
+      </c>
       <c r="H10" s="7" t="str">
         <f>VLOOKUP($D10,Table1[],4,FALSE)</f>
         <v>Template-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
@@ -2053,12 +2083,15 @@
         <f>VLOOKUP($D11,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G11" t="s">
+        <v>156</v>
+      </c>
       <c r="H11" s="7" t="str">
         <f>VLOOKUP($D11,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>104</v>
       </c>
@@ -2080,12 +2113,15 @@
         <f>VLOOKUP($D12,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
       <c r="H12" s="7" t="str">
         <f>VLOOKUP($D12,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>75</v>
       </c>
@@ -2107,12 +2143,15 @@
         <f>VLOOKUP($D13,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G13" t="s">
+        <v>156</v>
+      </c>
       <c r="H13" s="7" t="str">
         <f>VLOOKUP($D13,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>78</v>
       </c>
@@ -2134,51 +2173,54 @@
         <f>VLOOKUP($D14,Table1[],3,FALSE)</f>
         <v>0.19</v>
       </c>
+      <c r="G14" t="s">
+        <v>156</v>
+      </c>
       <c r="H14" s="7" t="str">
         <f>VLOOKUP($D14,Table1[],4,FALSE)</f>
         <v>Template-1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
   </sheetData>
@@ -2196,25 +2238,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB3F874-CC04-47A2-9677-58135BF38EE7}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.5234375" customWidth="1"/>
-    <col min="5" max="5" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +2289,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -2273,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>40</v>
       </c>
@@ -2296,7 +2338,7 @@
         <v>22500</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
@@ -2323,7 +2365,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2392,7 @@
         <v>488000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2419,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -2404,7 +2446,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -2436,7 +2478,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>47</v>
       </c>
@@ -2459,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>47</v>
       </c>
@@ -2482,7 +2524,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>47</v>
       </c>
@@ -2510,7 +2552,7 @@
       </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>47</v>
       </c>
@@ -2538,7 +2580,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -2561,7 +2603,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
@@ -2589,7 +2631,7 @@
       </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2614,7 +2656,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>57</v>
       </c>
@@ -2637,7 +2679,7 @@
         <v>41600</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
@@ -2660,7 +2702,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>57</v>
       </c>
@@ -2683,7 +2725,7 @@
         <v>15300</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>57</v>
       </c>
@@ -2708,7 +2750,7 @@
         <v>37000</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>57</v>
       </c>
@@ -2729,7 +2771,7 @@
       <c r="H20" s="10"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>57</v>
       </c>
@@ -2750,7 +2792,7 @@
       <c r="H21" s="10"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
@@ -2775,7 +2817,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>82</v>
       </c>
@@ -2798,7 +2840,7 @@
       <c r="H23" s="10"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>104</v>
       </c>
@@ -2824,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -2865,7 +2907,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2877,34 +2919,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2922,13 +2964,13 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.05078125" customWidth="1"/>
-    <col min="5" max="5" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>106</v>
       </c>
@@ -2942,7 +2984,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>107</v>
       </c>
@@ -2956,7 +2998,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>108</v>
       </c>
@@ -2967,7 +3009,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>109</v>
       </c>
@@ -2978,7 +3020,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>110</v>
       </c>

</xml_diff>